<commit_message>
Added Minifit Jr. to BOM
</commit_message>
<xml_diff>
--- a/Project/Task10/PDM_BOM.xlsx
+++ b/Project/Task10/PDM_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="70">
   <si>
     <t>Qty</t>
   </si>
@@ -47,6 +47,12 @@
     <t>5566-2</t>
   </si>
   <si>
+    <t>WM3875-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/0039299027/WM3875-ND/2002681</t>
+  </si>
+  <si>
     <t>BATT*</t>
   </si>
   <si>
@@ -80,7 +86,7 @@
     <t>C1206K</t>
   </si>
   <si>
-    <t>399-8269-1-ND </t>
+    <t>399-8269-1-ND</t>
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/T491A106K016AT/399-8269-1-ND/3471992</t>
@@ -110,7 +116,7 @@
     <t>SMBJ</t>
   </si>
   <si>
-    <t>SMBJ8.5ALFCT-ND </t>
+    <t>SMBJ8.5ALFCT-ND</t>
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/SMBJ8.5A/SMBJ8.5ALFCT-ND/762818</t>
@@ -128,7 +134,7 @@
     <t>SMB</t>
   </si>
   <si>
-    <t>1SMB5913BT3GOSCT-ND </t>
+    <t>1SMB5913BT3GOSCT-ND</t>
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/1SMB5913BT3G/1SMB5913BT3GOSCT-ND/917716</t>
@@ -146,7 +152,7 @@
     <t>ATO</t>
   </si>
   <si>
-    <t>WK6265-ND </t>
+    <t>WK6265-ND</t>
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/178.6165.0002/WK6265-ND/653477</t>
@@ -161,7 +167,7 @@
     <t>SML1206</t>
   </si>
   <si>
-    <t>160-1169-1-ND </t>
+    <t>160-1169-1-ND</t>
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/LTST-C150GKT/160-1169-1-ND/269241</t>
@@ -179,7 +185,7 @@
     <t>R1206</t>
   </si>
   <si>
-    <t>RMCF1206JT1K00CT-ND </t>
+    <t>RMCF1206JT1K00CT-ND</t>
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/RMCF1206JT1K00/RMCF1206JT1K00CT-ND/1942786</t>
@@ -191,7 +197,7 @@
     <t>15.4K 1% Tolerance</t>
   </si>
   <si>
-    <t>RMCF1206FT15K4CT-ND </t>
+    <t>RMCF1206FT15K4CT-ND</t>
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/RMCF1206FT15K4/RMCF1206FT15K4CT-ND/2418587</t>
@@ -228,11 +234,12 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -254,6 +261,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -311,12 +326,16 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -408,7 +427,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A14" activeCellId="0" pane="topLeft" sqref="A14"/>
+      <selection activeCell="F3" activeCellId="0" pane="topLeft" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -461,25 +480,31 @@
       <c r="E2" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="4">
@@ -487,19 +512,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="5">
@@ -507,22 +532,22 @@
         <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="6">
@@ -530,22 +555,22 @@
         <v>2</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
@@ -553,22 +578,22 @@
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="8">
@@ -576,22 +601,22 @@
         <v>1</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="9">
@@ -599,22 +624,22 @@
         <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
@@ -622,19 +647,19 @@
         <v>6</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="11">
@@ -642,22 +667,22 @@
         <v>6</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="12">
@@ -665,22 +690,22 @@
         <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="13">
@@ -688,48 +713,51 @@
         <v>1</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="14">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
+      <c r="A14" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink display="http://www.digikey.com/product-detail/en/0039299027/WM3875-ND/2002681" ref="G2" r:id="rId1"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>

</xml_diff>

<commit_message>
Updated Solidworks to begin assembly
</commit_message>
<xml_diff>
--- a/Project/Task10/PDM_BOM.xlsx
+++ b/Project/Task10/PDM_BOM.xlsx
@@ -427,7 +427,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F3" activeCellId="0" pane="topLeft" sqref="F3"/>
+      <selection activeCell="A14" activeCellId="0" pane="topLeft" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -469,7 +469,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>7</v>
@@ -487,9 +487,9 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>12</v>
@@ -509,7 +509,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>16</v>
@@ -529,7 +529,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>19</v>
@@ -552,7 +552,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="6">
       <c r="A6" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>25</v>
@@ -575,7 +575,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
       <c r="A7" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>29</v>
@@ -598,7 +598,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="8">
       <c r="A8" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>35</v>
@@ -621,7 +621,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="9">
       <c r="A9" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>41</v>
@@ -644,7 +644,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
       <c r="A10" s="0" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>47</v>
@@ -664,7 +664,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="11">
       <c r="A11" s="0" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>52</v>
@@ -687,7 +687,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="12">
       <c r="A12" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>58</v>
@@ -710,7 +710,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="13">
       <c r="A13" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>62</v>

</xml_diff>